<commit_message>
9.1.5 spreadsheet filled out
</commit_message>
<xml_diff>
--- a/Stat Breakdown.xlsx
+++ b/Stat Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Darkshore Capital\Git\mythic-plus-toolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE033FAB-F237-4C8C-85B7-C41D23FFE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9331FFA0-ADA2-4C80-BF33-B0261AA15128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="915" windowWidth="27450" windowHeight="17355" xr2:uid="{2F668EE4-BA2E-4273-8EDF-2287691078C0}"/>
+    <workbookView xWindow="11550" yWindow="840" windowWidth="23580" windowHeight="16845" xr2:uid="{2F668EE4-BA2E-4273-8EDF-2287691078C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="77">
   <si>
     <t>Class</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>Lightless Force</t>
+  </si>
+  <si>
+    <t>Fortified Speed</t>
+  </si>
+  <si>
+    <t>30 Stamina</t>
   </si>
 </sst>
 </file>
@@ -614,11 +620,12 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
@@ -1066,13 +1073,19 @@
         <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
         <v>59</v>
       </c>
       <c r="H18" t="s">
         <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1082,8 +1095,20 @@
       <c r="E19" t="s">
         <v>54</v>
       </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
       <c r="H19" t="s">
         <v>70</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1096,8 +1121,20 @@
       <c r="E20" t="s">
         <v>55</v>
       </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
       <c r="H20" t="s">
         <v>70</v>
+      </c>
+      <c r="I20" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1107,8 +1144,20 @@
       <c r="E21" t="s">
         <v>53</v>
       </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
       <c r="H21" t="s">
         <v>70</v>
+      </c>
+      <c r="I21" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1118,8 +1167,20 @@
       <c r="E22" t="s">
         <v>53</v>
       </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
       <c r="H22" t="s">
         <v>70</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1141,6 +1202,12 @@
       <c r="H23" t="s">
         <v>70</v>
       </c>
+      <c r="I23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
@@ -1149,11 +1216,20 @@
       <c r="E24" t="s">
         <v>55</v>
       </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
       <c r="G24" t="s">
         <v>59</v>
       </c>
       <c r="H24" t="s">
         <v>70</v>
+      </c>
+      <c r="I24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1163,11 +1239,20 @@
       <c r="E25" t="s">
         <v>55</v>
       </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
       <c r="G25" t="s">
         <v>59</v>
       </c>
       <c r="H25" t="s">
         <v>70</v>
+      </c>
+      <c r="I25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1180,8 +1265,23 @@
       <c r="E26" t="s">
         <v>54</v>
       </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
       <c r="H26" t="s">
         <v>70</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1191,8 +1291,23 @@
       <c r="E27" t="s">
         <v>54</v>
       </c>
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
       <c r="H27" t="s">
         <v>70</v>
+      </c>
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1202,8 +1317,23 @@
       <c r="E28" t="s">
         <v>54</v>
       </c>
+      <c r="F28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" t="s">
+        <v>62</v>
+      </c>
       <c r="H28" t="s">
         <v>70</v>
+      </c>
+      <c r="I28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1216,11 +1346,20 @@
       <c r="E29" t="s">
         <v>55</v>
       </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
       <c r="G29" t="s">
         <v>59</v>
       </c>
       <c r="H29" t="s">
         <v>70</v>
+      </c>
+      <c r="I29" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1230,8 +1369,23 @@
       <c r="E30" t="s">
         <v>54</v>
       </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>58</v>
+      </c>
       <c r="H30" t="s">
         <v>70</v>
+      </c>
+      <c r="I30" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K30" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1250,6 +1404,12 @@
       <c r="H31" t="s">
         <v>70</v>
       </c>
+      <c r="I31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -1261,42 +1421,69 @@
       <c r="E32" t="s">
         <v>55</v>
       </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
       <c r="G32" t="s">
         <v>59</v>
       </c>
       <c r="H32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>48</v>
       </c>
       <c r="E33" t="s">
         <v>55</v>
       </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
       <c r="G33" t="s">
         <v>59</v>
       </c>
       <c r="H33" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>76</v>
+      </c>
+      <c r="J33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>49</v>
       </c>
       <c r="E34" t="s">
         <v>55</v>
       </c>
+      <c r="F34" t="s">
+        <v>71</v>
+      </c>
       <c r="G34" t="s">
         <v>59</v>
       </c>
       <c r="H34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -1306,30 +1493,69 @@
       <c r="E35" t="s">
         <v>53</v>
       </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>62</v>
+      </c>
       <c r="H35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>52</v>
       </c>
       <c r="E36" t="s">
         <v>53</v>
       </c>
+      <c r="F36" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" t="s">
+        <v>62</v>
+      </c>
       <c r="H36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>61</v>
+      </c>
+      <c r="J36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>28</v>
       </c>
       <c r="E37" t="s">
         <v>53</v>
       </c>
+      <c r="F37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
       <c r="H37" t="s">
         <v>70</v>
+      </c>
+      <c r="I37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Combat Rogue, Fix Brewmaster
</commit_message>
<xml_diff>
--- a/Stat Breakdown.xlsx
+++ b/Stat Breakdown.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Darkshore Capital\Git\mythic-plus-toolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9331FFA0-ADA2-4C80-BF33-B0261AA15128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C1803C-46F5-4F64-BDBE-9C301923A05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="840" windowWidth="23580" windowHeight="16845" xr2:uid="{2F668EE4-BA2E-4273-8EDF-2287691078C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2F668EE4-BA2E-4273-8EDF-2287691078C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="9.1.5" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'9.1.5'!$B$1:$K$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -281,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -301,8 +307,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +627,8 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,130 +678,130 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="K5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="H6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -846,26 +854,26 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1088,52 +1096,52 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="19" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="H19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="J19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="G20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1183,29 +1191,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G23" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="G23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1388,26 +1396,26 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="31" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G31" t="s">
-        <v>59</v>
-      </c>
-      <c r="H31" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="G31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="1" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>